<commit_message>
Changes made in LogInTest Class
</commit_message>
<xml_diff>
--- a/7rmartPro1/src/main/resources/TestData.xlsx
+++ b/7rmartPro1/src/main/resources/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\git\SeleniumProjects\7rmartPro1\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139A9206-A37D-4114-BA07-33A9F4248B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3400A693-F0C3-4EE5-A7F3-7E08AA5A5614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4044" yWindow="1056" windowWidth="17280" windowHeight="11184" xr2:uid="{864BBC4D-16B3-49E8-B0CD-A0732A24B301}"/>
   </bookViews>
@@ -34,15 +34,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
-  <si>
-    <t>Correct username</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>admin</t>
   </si>
   <si>
-    <t>Correct password</t>
+    <t>Invaid Username</t>
+  </si>
+  <si>
+    <t>invalidUsername</t>
+  </si>
+  <si>
+    <t>Invalid Password</t>
+  </si>
+  <si>
+    <t>invalidPassword</t>
+  </si>
+  <si>
+    <t>Correct Username</t>
+  </si>
+  <si>
+    <t>Correct Password</t>
   </si>
 </sst>
 </file>
@@ -394,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D4A6D8-221E-4B05-8210-0DA66C75F79E}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,18 +420,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 3 new TCs
</commit_message>
<xml_diff>
--- a/7rmartPro1/src/main/resources/TestData.xlsx
+++ b/7rmartPro1/src/main/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\git\SeleniumProjects\7rmartPro1\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F893C6-CE66-4F4D-80FE-167D8DB95F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BFCBD7-2CCB-40F1-8921-7699B2251C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="922" activeTab="2" xr2:uid="{864BBC4D-16B3-49E8-B0CD-A0732A24B301}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
   <si>
     <t>admin</t>
   </si>
@@ -156,18 +156,9 @@
     <t>Manage Offer Code</t>
   </si>
   <si>
-    <t>X100RIZZ</t>
-  </si>
-  <si>
     <t>New Year Offer</t>
   </si>
   <si>
-    <t xml:space="preserve">  offerCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  percentage </t>
-  </si>
-  <si>
     <t xml:space="preserve">  description</t>
   </si>
   <si>
@@ -184,6 +175,12 @@
   </si>
   <si>
     <t>Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  percentage</t>
+  </si>
+  <si>
+    <t>Manage Delivery Boy</t>
   </si>
 </sst>
 </file>
@@ -664,10 +661,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF28234E-F15D-4D68-9F03-5B8CFEEEB836}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,8 +690,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -861,7 +867,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -896,19 +902,14 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" t="s">
-        <v>38</v>
+        <v>45</v>
+      </c>
+      <c r="B4">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.3</v>
-      </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -920,10 +921,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -966,23 +967,23 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added listeners, retry and ss classes
</commit_message>
<xml_diff>
--- a/7rmartPro1/src/main/resources/TestData.xlsx
+++ b/7rmartPro1/src/main/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\git\SeleniumProjects\7rmartPro1\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F68B41D-49D3-46CF-88A3-9F8141FCAA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956EA6E3-FC49-4023-AAAC-015637CEB563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="922" activeTab="6" xr2:uid="{864BBC4D-16B3-49E8-B0CD-A0732A24B301}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="922" xr2:uid="{864BBC4D-16B3-49E8-B0CD-A0732A24B301}"/>
   </bookViews>
   <sheets>
     <sheet name="LogIn" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
   <si>
     <t>admin</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>jack</t>
+  </si>
+  <si>
+    <t>adminYadhu</t>
   </si>
 </sst>
 </file>
@@ -557,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D4A6D8-221E-4B05-8210-0DA66C75F79E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -572,7 +575,7 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -954,7 +957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15A92E1-394C-45A6-8145-56D1892BC57F}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added xml files for grouping and parallel testing
</commit_message>
<xml_diff>
--- a/7rmartPro1/src/main/resources/TestData.xlsx
+++ b/7rmartPro1/src/main/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\git\SeleniumProjects\7rmartPro1\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956EA6E3-FC49-4023-AAAC-015637CEB563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB41238-61BD-47F1-8A3E-46E86647F01D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="922" xr2:uid="{864BBC4D-16B3-49E8-B0CD-A0732A24B301}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
   <si>
     <t>admin</t>
   </si>
@@ -203,9 +203,6 @@
   </si>
   <si>
     <t>jack</t>
-  </si>
-  <si>
-    <t>adminYadhu</t>
   </si>
 </sst>
 </file>
@@ -575,7 +572,7 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>